<commit_message>
Sửa sơ đồ Grantt, biểu đồ phụ tải
</commit_message>
<xml_diff>
--- a/Documents/QLDA/Thời_gian_dự_trữ.xlsx
+++ b/Documents/QLDA/Thời_gian_dự_trữ.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Công việc</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Q</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -451,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,13 +498,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
@@ -512,16 +515,16 @@
         <v>7</v>
       </c>
       <c r="B3" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D3" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
@@ -532,16 +535,16 @@
         <v>8</v>
       </c>
       <c r="B4" s="2">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C4" s="2">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D4" s="2">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E4" s="2">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
@@ -552,16 +555,16 @@
         <v>9</v>
       </c>
       <c r="B5" s="2">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="D5" s="2">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E5" s="2">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F5" s="2">
         <v>0</v>
@@ -572,16 +575,16 @@
         <v>10</v>
       </c>
       <c r="B6" s="2">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C6" s="2">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D6" s="2">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E6" s="2">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="F6" s="2">
         <v>0</v>
@@ -592,16 +595,16 @@
         <v>11</v>
       </c>
       <c r="B7" s="2">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="C7" s="2">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="D7" s="2">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
@@ -612,19 +615,19 @@
         <v>12</v>
       </c>
       <c r="B8" s="2">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D8" s="2">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="E8" s="2">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="F8" s="2">
-        <v>18</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
@@ -632,19 +635,19 @@
         <v>13</v>
       </c>
       <c r="B9" s="2">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="D9" s="2">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="E9" s="2">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="F9" s="2">
-        <v>0</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
@@ -652,16 +655,16 @@
         <v>14</v>
       </c>
       <c r="B10" s="2">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C10" s="2">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="D10" s="2">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="E10" s="2">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="F10" s="2">
         <v>0</v>
@@ -672,19 +675,19 @@
         <v>15</v>
       </c>
       <c r="B11" s="2">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C11" s="2">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="D11" s="2">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="E11" s="2">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="F11" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
@@ -692,16 +695,16 @@
         <v>16</v>
       </c>
       <c r="B12" s="2">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="C12" s="2">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="D12" s="2">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="E12" s="2">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="F12" s="2">
         <v>2</v>
@@ -712,19 +715,19 @@
         <v>17</v>
       </c>
       <c r="B13" s="2">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="C13" s="2">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="D13" s="2">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="E13" s="2">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="F13" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
@@ -732,19 +735,19 @@
         <v>19</v>
       </c>
       <c r="B14" s="2">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="C14" s="2">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="D14" s="2">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="E14" s="2">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="F14" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
@@ -752,19 +755,19 @@
         <v>18</v>
       </c>
       <c r="B15" s="2">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="C15" s="2">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="D15" s="2">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="E15" s="2">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="F15" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
@@ -772,16 +775,16 @@
         <v>20</v>
       </c>
       <c r="B16" s="2">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="C16" s="2">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="D16" s="2">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="E16" s="2">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="F16" s="2">
         <v>0</v>
@@ -792,16 +795,16 @@
         <v>21</v>
       </c>
       <c r="B17" s="2">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="C17" s="2">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="D17" s="2">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="E17" s="2">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="F17" s="2">
         <v>0</v>
@@ -812,18 +815,38 @@
         <v>22</v>
       </c>
       <c r="B18" s="2">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="C18" s="2">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="D18" s="2">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="E18" s="2">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="F18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="2">
+        <v>73</v>
+      </c>
+      <c r="C19" s="2">
+        <v>78</v>
+      </c>
+      <c r="D19" s="2">
+        <v>73</v>
+      </c>
+      <c r="E19" s="2">
+        <v>78</v>
+      </c>
+      <c r="F19" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>